<commit_message>
feature udistrital/sga_documentacion#136 Finalización reporte inscritos
Se corrige la devolución de un base64 muy grande debido a la calidad de el header que se agregaba al reporte, se finaliza el primer reporte
</commit_message>
<xml_diff>
--- a/static/templates/ReporteInscritosOriginal.xlsx
+++ b/static/templates/ReporteInscritosOriginal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\moreraz\go\src\github.com\udistrital\sga_admisiones_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162042AF-B0C1-4A15-87E8-3D35FBD183BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EADC7-403E-4C22-9B7E-01B98493F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,11 +98,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -110,7 +136,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -427,49 +456,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FB3C54-1B50-4EEB-8DFE-F1FD6F4DDA94}">
-  <dimension ref="A2:I5"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="2" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+    <row r="3" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -480,38 +509,62 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Feature udistrital/sga_documentacion#136 Adicion segundo reporte, con fallos
</commit_message>
<xml_diff>
--- a/static/templates/ReporteInscritosOriginal.xlsx
+++ b/static/templates/ReporteInscritosOriginal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\moreraz\go\src\github.com\udistrital\sga_admisiones_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EADC7-403E-4C22-9B7E-01B98493F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA5531-B5B2-4E2D-8F41-6BC08459A832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
+    <workbookView xWindow="5760" yWindow="3990" windowWidth="21600" windowHeight="11385" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,35 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Número Documento</t>
-  </si>
-  <si>
-    <t>Nombre Completo</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
-    <t>Credencial</t>
-  </si>
-  <si>
-    <t>Enfasis</t>
-  </si>
-  <si>
-    <t>Descuento</t>
-  </si>
-  <si>
-    <t>Estado inscripción</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -128,9 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -139,7 +114,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,106 +437,88 @@
   <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+    <row r="2" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+    <row r="3" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+    <row r="5" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>8</v>
-      </c>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Feat: cambio plantilla udistrital/sga_documentacion#164
Se cambia la plantilla para abarcar todos los campos que requiere el reporte de aspirantes para todos los proyectos
</commit_message>
<xml_diff>
--- a/static/templates/ReporteInscritosOriginal.xlsx
+++ b/static/templates/ReporteInscritosOriginal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\moreraz\go\src\github.com\udistrital\sga_admisiones_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA5531-B5B2-4E2D-8F41-6BC08459A832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B709E224-92BB-4E90-B942-E49AA88CA07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3990" windowWidth="21600" windowHeight="11385" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71686BF1-9572-4690-90F1-53D04F458C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,54 +66,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -434,49 +401,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FB3C54-1B50-4EEB-8DFE-F1FD6F4DDA94}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="2" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+    <row r="3" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -486,30 +455,33 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -519,12 +491,13 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A2:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>

</xml_diff>